<commit_message>
2010-11-30 - Cleaning up.
</commit_message>
<xml_diff>
--- a/RIS_spec_overview.xlsx
+++ b/RIS_spec_overview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="25600" windowHeight="14360" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="25600" windowHeight="14360" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RIS fields" sheetId="1" r:id="rId1"/>
@@ -4213,7 +4213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A57" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A57" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
@@ -6205,7 +6205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
@@ -6978,7 +6978,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7021,8 +7020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E476"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView showRuler="0" topLeftCell="A433" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15126,7 +15125,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D476">
+  <sortState ref="A2:E476">
     <sortCondition ref="A2:A476"/>
     <sortCondition ref="B2:B476"/>
   </sortState>
@@ -15143,7 +15142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1793"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A395" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A1634" workbookViewId="0">
       <selection activeCell="B1666" sqref="B1666"/>
     </sheetView>
   </sheetViews>

</xml_diff>